<commit_message>
CAN code issues with the initialization
</commit_message>
<xml_diff>
--- a/Documentation/Project Logbook.xlsx
+++ b/Documentation/Project Logbook.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepoGitSVN\AEP_PSS_ACU\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uidn8311\Desktop\Final Project Workspace\AEP_PSS_ACU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
   <si>
     <t>Start Date</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>Code compatibiity and folder structure issues fixed</t>
+  </si>
+  <si>
+    <t>Antonio Vazquez</t>
+  </si>
+  <si>
+    <t>CAN code issues with the initialization solved (still present some problems with the timer)</t>
   </si>
 </sst>
 </file>
@@ -366,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -439,6 +445,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -779,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D875"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="C32" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,7 +1260,20 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="26">
+        <v>43080</v>
+      </c>
+      <c r="B40" s="26">
+        <v>43080</v>
+      </c>
+      <c r="C40" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>